<commit_message>
Fix bug in RNN_test in 2b
</commit_message>
<xml_diff>
--- a/homework/hw7/NLP.xlsx
+++ b/homework/hw7/NLP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziyu/Library/Containers/com.microsoft.Excel/Data/Desktop/Study Affairs/2018-Fall/cs598-deep-learning/homework/hw7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE0AA3F-3D7A-3A4B-9A8F-678E967A0CD2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153E9A24-556A-EE4B-8765-3289EE272D94}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="0" windowWidth="19600" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="200" windowWidth="22020" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Natural Language Processing - IMDB Movie Review</t>
   </si>
@@ -115,15 +115,9 @@
     <t>ADAM optimizer with LR=0.001, BatchSize=200, VocabularySize=100000, HiddenUnits=500, SequenceLengthOfTrain=100, SequenceLengthOfTest=100</t>
   </si>
   <si>
-    <t>ADAM optimizer with LR=0.001, BatchSize=200, VocabularySize=8000, HiddenUnits=500, SequenceLengthOfTrain=100, SequenceLengthOfTest=100</t>
-  </si>
-  <si>
     <t>84.82%. ~91%</t>
   </si>
   <si>
-    <t>81.94% ~87%</t>
-  </si>
-  <si>
     <t>ADAM optimizer with LR=0.001, BatchSize=200, VocabularySize=8000, HiddenUnits=1000</t>
   </si>
   <si>
@@ -143,6 +137,15 @@
   </si>
   <si>
     <t>The number of hidden units is decreased to 10 to make the model underfit. The training accuracy decreases by 3%, while the test accuracy doesn't change much. Despite its purpose, this change seems to alleviate the overfitting problem of the original model. A possible reason is that the function we want to approximate using our network is not that complex so making the model simpler won't hurt the performance.</t>
+  </si>
+  <si>
+    <t>ADAM optimizer with LR=0.001, BatchSize=200, VocabularySize=8000, HiddenUnits=500, SequenceLengthOfTrain=100, SequenceLengthOfTest=400</t>
+  </si>
+  <si>
+    <t>ADAM optimizer with LR=0.001, BatchSize=200, VocabularySize=8000, HiddenUnits=500, SequenceLengthOfTrain=400, SequenceLengthOfTest=400</t>
+  </si>
+  <si>
+    <t>The sequence length for training is increased from 100 to 400. The model is now overfitting. Training accuracy is approaching 100% while test accuracy is only 79.07%, which is worse than the given model.</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -611,7 +614,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
@@ -626,7 +629,7 @@
         <v>0.86070000000000002</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="39">
@@ -634,7 +637,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4">
         <v>6</v>
@@ -649,7 +652,7 @@
         <v>0.83240000000000003</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13">
@@ -693,7 +696,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
@@ -708,7 +711,7 @@
         <v>0.84519999999999995</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65">
@@ -717,7 +720,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4">
         <v>6</v>
@@ -732,7 +735,7 @@
         <v>0.85340000000000005</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13">
@@ -765,7 +768,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4">
         <v>20</v>
@@ -776,22 +779,34 @@
       <c r="F13" s="10">
         <v>0.9637</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>33</v>
+      <c r="G13" s="5">
+        <v>0.87690000000000001</v>
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="13">
+    <row r="14" spans="1:8" ht="65">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="4">
+        <v>20</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.99429999999999996</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.79069999999999996</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="13">
       <c r="A15" s="4"/>
@@ -847,7 +862,7 @@
         <v>0.91520000000000001</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="4"/>
     </row>

</xml_diff>